<commit_message>
Application: Download: Add SpeedyPage
</commit_message>
<xml_diff>
--- a/Application/Download.xlsx
+++ b/Application/Download.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="77">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -249,6 +249,54 @@
   </si>
   <si>
     <t>刚部署的原因？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云北京H - Tokyo - SpeedyPage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Azure JP - Tokyo - SpeedyPage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.7ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>China - Azure JP - Tokyo - SpeedPage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>130.7ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云北京H - Singapore - SpeedyPage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>125ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云北京H - Los Angeles - SpeedyPage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>280ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云北京H - Ashburn - SpeedyPage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>275ms</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -522,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2675,7 +2723,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B145" s="2">
         <v>0.82152777777777775</v>
       </c>
@@ -2689,7 +2737,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B146" s="2">
         <v>0.8222222222222223</v>
       </c>
@@ -2703,7 +2751,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B147" s="2">
         <v>0.82430555555555562</v>
       </c>
@@ -2715,6 +2763,102 @@
       </c>
       <c r="F147" s="3">
         <v>10.9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A148" s="1">
+        <v>45728</v>
+      </c>
+      <c r="B148" s="2">
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="C148" t="s">
+        <v>65</v>
+      </c>
+      <c r="D148" t="s">
+        <v>66</v>
+      </c>
+      <c r="F148" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B149" s="2">
+        <v>0.82986111111111116</v>
+      </c>
+      <c r="C149" t="s">
+        <v>67</v>
+      </c>
+      <c r="D149" t="s">
+        <v>10</v>
+      </c>
+      <c r="F149" s="3">
+        <v>66.2</v>
+      </c>
+      <c r="I149" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B150" s="2">
+        <v>0.83819444444444446</v>
+      </c>
+      <c r="C150" t="s">
+        <v>69</v>
+      </c>
+      <c r="I150" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B151" s="2">
+        <v>0.85277777777777775</v>
+      </c>
+      <c r="C151" t="s">
+        <v>71</v>
+      </c>
+      <c r="D151" t="s">
+        <v>10</v>
+      </c>
+      <c r="F151" s="3">
+        <v>5.94</v>
+      </c>
+      <c r="I151" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B152" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C152" t="s">
+        <v>73</v>
+      </c>
+      <c r="D152" t="s">
+        <v>10</v>
+      </c>
+      <c r="F152" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="I152" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B153" s="2">
+        <v>0.85555555555555562</v>
+      </c>
+      <c r="C153" t="s">
+        <v>75</v>
+      </c>
+      <c r="D153" t="s">
+        <v>10</v>
+      </c>
+      <c r="F153" s="3">
+        <v>1.26</v>
+      </c>
+      <c r="I153" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Application: Download: Update xlsx
</commit_message>
<xml_diff>
--- a/Application/Download.xlsx
+++ b/Application/Download.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="188">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -297,6 +297,427 @@
   </si>
   <si>
     <t>275ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - Azure JP - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云北京H - Azure JP - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云北京H - 阿里云DCDN Range - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - 多吉云 Range - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云北京H - 多吉云 Range - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - Hysteria BBR - Azure JP - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - Hysteria BBR - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - CMIN2 - Seattle Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT - AS4837 - Hysteria BBR - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT - AS4837 - Hysteria Brutal 200M - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT - CMIN2 - Seattle Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - quiche-server BBR - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curl --insecure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - h3-quinn BBR - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - h3-quinn BBR ACK 10 MTU 1460 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - Hysteria masq - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - Hysteria masq BBR - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - Hysteria masq Brutal 100M - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - Hysteria masq proxy Brutal 100M - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - 阿里云OSS 香港</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - 阿里云OSS 香港 传输加速</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT - 阿里云OSS 上海</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火山引擎 北京 - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云 北京H - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hysteria</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - 快车道 香港BGP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iOS Safari</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AkileCloud JPPro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - AS4837 - AkileCloud JPPro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - AS4837 - AkileCloud JPHyper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AkileCloud JPHyper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - AS4837 - Hetzner DE Falkenstein</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>155ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - Hetzner DE Falkenstein</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>207ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>166ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - Seattle Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speedtest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AnyTLS - AS4837 - CUBIC - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - Hysteria 200M - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - Hysteria Brutal 200/30M - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AS4837 - Seattle</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AS4837 - BBR - Seattle Test</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AS4837 - Hysteria BBR - Seattle</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AS4837 - Hysteria Brutal 100M - Seattle</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AS4837 - Hysteria Brutal 200M - Seattle</t>
+  </si>
+  <si>
+    <t>CM - CUBIC - 阿里云轻量 上海139.224</t>
+  </si>
+  <si>
+    <t>CM - BBR - 阿里云轻量 上海139.224</t>
+  </si>
+  <si>
+    <t>CT - BBR - 阿里云轻量 上海139.224</t>
+  </si>
+  <si>
+    <t>CM - 阿里云轻量 上海139.224 - AS4837 - Hysteria BBR - Seattle</t>
+  </si>
+  <si>
+    <t>CT - 阿里云轻量 上海139.224 - AS4837 - Hysteria BBR - Seattle</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - CMIN2 - Seattle Test</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AS4837 - Seattle Test</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AkileCloud JPHyper</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AS4837 - CUBIC - Seattle</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AS4837 - Hysteria Brutal 150M - Seattle</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AkileCloud JPPro</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AkileCloud JPIIJ</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AkileCloud HKLite</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AkileCloud LAX4837</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AkileCloud LaxPro</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - AkileCloud SGLite</t>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - Hetzner DE Falkenstein</t>
+  </si>
+  <si>
+    <t>CM - AnyTLS - 阿里云轻量 上海139.224 - Hysteria 150M - AS4837 - Seattle</t>
+  </si>
+  <si>
+    <t>CM - AnyTLS - 阿里云轻量 上海47.117 - Hysteria 150M - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云轻量 上海139.224 - Hetzner DE Falkenstein</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - AS4837 - BBR - 阿里云轻量 上海47.117</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - AS4837 - BBR - 阿里云轻量 上海47.117 - Hysteria Brutal 150M - AS4837 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tusd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - AS4837 - Hysteria 30M - 阿里云轻量 上海47.117 - CM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云轻量 上海47.117 - CM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云轻量 上海47.117 - CT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - AS4837  - 阿里云轻量 上海47.117 - CM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - AS4837  - CM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - AS4837 - 阿里云轻量 上海47.117 - CM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - RFCHost HKG-CMI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - RFCHost TYO-T1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - 4837/CMI - RFCHost TYO-CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - RFCHost HKG-T1-CTC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - RFCHost HKG-T1-JINX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - RFCHost LAX-CN2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - RFCHost LAX-T1-Classic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - RFCHost SGP-T1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT - RFCHost HKG-CMI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - RFCHost HKG-CMI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - RFCHost TYO-CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle - RFCHost LAX-T1-Classic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - Seattle Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - Hysteria BBR - AS4837 - Seattle - RFCHost HKG-CMI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - Hysteria BBR - AS4837 - Seattle - 4837/CMI - RFCHost TYO-CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT - 4837/CMI - RFCHost TYO-CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT - RFCHost TYO-T1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CM - AS4837 - BBR2 - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云轻量 广州8.138 - AS4837 - BBR - Seattle Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云轻量 上海47.116 - AS4837 - BBR - Seattle Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里云轻量 广州8.138 - AS4837 - Hysteria 150M - Seattle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>173ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>174ms, HTTP +30ms?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT - AS9929 - Seattle Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT - AS4837 - BBR - Seattle Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -570,18 +991,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:I349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="D156" sqref="D156"/>
+    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
+      <selection activeCell="I347" sqref="I347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="53.44140625" customWidth="1"/>
+    <col min="3" max="3" width="54.109375" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
     <col min="6" max="6" width="8" style="3" customWidth="1"/>
     <col min="7" max="7" width="6.5546875" hidden="1" customWidth="1"/>
@@ -2861,23 +3282,3010 @@
         <v>76</v>
       </c>
     </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A154" s="1">
+        <v>45740</v>
+      </c>
+      <c r="B154" s="2">
+        <v>0.93333333333333324</v>
+      </c>
+      <c r="C154" t="s">
+        <v>26</v>
+      </c>
+      <c r="D154" t="s">
+        <v>77</v>
+      </c>
+      <c r="F154" s="3">
+        <v>0.623</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B155" s="2">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="C155" t="s">
+        <v>78</v>
+      </c>
+      <c r="D155" t="s">
+        <v>10</v>
+      </c>
+      <c r="F155" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B156" s="2">
+        <v>0.93541666666666667</v>
+      </c>
+      <c r="C156" t="s">
+        <v>53</v>
+      </c>
+      <c r="D156" t="s">
+        <v>10</v>
+      </c>
+      <c r="F156" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B157" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="C157" t="s">
+        <v>28</v>
+      </c>
+      <c r="D157" t="s">
+        <v>10</v>
+      </c>
+      <c r="F157" s="3">
+        <v>10</v>
+      </c>
+      <c r="I157" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B158" s="2">
+        <v>0.93819444444444444</v>
+      </c>
+      <c r="C158" t="s">
+        <v>80</v>
+      </c>
+      <c r="D158" t="s">
+        <v>10</v>
+      </c>
+      <c r="F158" s="3">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B159" s="2">
+        <v>0.93888888888888899</v>
+      </c>
+      <c r="C159" t="s">
+        <v>81</v>
+      </c>
+      <c r="D159" t="s">
+        <v>10</v>
+      </c>
+      <c r="F159" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B160" s="2">
+        <v>0.94236111111111109</v>
+      </c>
+      <c r="C160" t="s">
+        <v>82</v>
+      </c>
+      <c r="D160" t="s">
+        <v>10</v>
+      </c>
+      <c r="F160" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B161" s="2">
+        <v>0.94444444444444453</v>
+      </c>
+      <c r="C161" t="s">
+        <v>83</v>
+      </c>
+      <c r="D161" t="s">
+        <v>10</v>
+      </c>
+      <c r="F161" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B162" s="2">
+        <v>0.94513888888888886</v>
+      </c>
+      <c r="C162" t="s">
+        <v>84</v>
+      </c>
+      <c r="D162" t="s">
+        <v>10</v>
+      </c>
+      <c r="F162" s="3">
+        <v>13</v>
+      </c>
+      <c r="I162" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B163" s="2">
+        <v>0.9458333333333333</v>
+      </c>
+      <c r="C163" t="s">
+        <v>85</v>
+      </c>
+      <c r="D163" t="s">
+        <v>10</v>
+      </c>
+      <c r="F163" s="3">
+        <v>10.7</v>
+      </c>
+      <c r="I163" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B164" s="2">
+        <v>0.9472222222222223</v>
+      </c>
+      <c r="C164" t="s">
+        <v>87</v>
+      </c>
+      <c r="D164" t="s">
+        <v>19</v>
+      </c>
+      <c r="F164" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="I164" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B165" s="2">
+        <v>0.94861111111111107</v>
+      </c>
+      <c r="C165" t="s">
+        <v>89</v>
+      </c>
+      <c r="D165" t="s">
+        <v>19</v>
+      </c>
+      <c r="F165" s="3">
+        <v>8</v>
+      </c>
+      <c r="I165" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B166" s="2">
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="C166" t="s">
+        <v>86</v>
+      </c>
+      <c r="D166" t="s">
+        <v>10</v>
+      </c>
+      <c r="F166" s="3">
+        <v>11.1</v>
+      </c>
+      <c r="I166" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B167" s="2">
+        <v>0.95277777777777783</v>
+      </c>
+      <c r="C167" t="s">
+        <v>90</v>
+      </c>
+      <c r="D167" t="s">
+        <v>19</v>
+      </c>
+      <c r="F167" s="3">
+        <v>10</v>
+      </c>
+      <c r="I167" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B168" s="2">
+        <v>0.9604166666666667</v>
+      </c>
+      <c r="C168" t="s">
+        <v>26</v>
+      </c>
+      <c r="D168" t="s">
+        <v>77</v>
+      </c>
+      <c r="F168" s="3">
+        <v>6.58</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B169" s="2">
+        <v>0.96111111111111114</v>
+      </c>
+      <c r="C169" t="s">
+        <v>26</v>
+      </c>
+      <c r="D169" t="s">
+        <v>77</v>
+      </c>
+      <c r="F169" s="3">
+        <v>7.98</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B170" s="2">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="C170" t="s">
+        <v>26</v>
+      </c>
+      <c r="D170" t="s">
+        <v>12</v>
+      </c>
+      <c r="F170" s="3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B171" s="2">
+        <v>0.96388888888888891</v>
+      </c>
+      <c r="C171" t="s">
+        <v>26</v>
+      </c>
+      <c r="D171" t="s">
+        <v>21</v>
+      </c>
+      <c r="F171" s="3">
+        <v>0.58399999999999996</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B172" s="2">
+        <v>0.96458333333333324</v>
+      </c>
+      <c r="C172" t="s">
+        <v>26</v>
+      </c>
+      <c r="D172" t="s">
+        <v>10</v>
+      </c>
+      <c r="F172" s="3">
+        <v>8.76</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B173" s="2">
+        <v>0.98888888888888893</v>
+      </c>
+      <c r="C173" t="s">
+        <v>26</v>
+      </c>
+      <c r="D173" t="s">
+        <v>10</v>
+      </c>
+      <c r="F173" s="3">
+        <v>6.87</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A174" s="1">
+        <v>45741</v>
+      </c>
+      <c r="B174" s="2">
+        <v>3.9583333333333331E-2</v>
+      </c>
+      <c r="C174" t="s">
+        <v>91</v>
+      </c>
+      <c r="D174" t="s">
+        <v>24</v>
+      </c>
+      <c r="F174" s="3">
+        <v>2.452</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B175" s="2">
+        <v>4.027777777777778E-2</v>
+      </c>
+      <c r="C175" t="s">
+        <v>93</v>
+      </c>
+      <c r="D175" t="s">
+        <v>92</v>
+      </c>
+      <c r="F175" s="3">
+        <v>5.2370000000000001</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B176" s="2">
+        <v>7.5694444444444439E-2</v>
+      </c>
+      <c r="C176" t="s">
+        <v>94</v>
+      </c>
+      <c r="D176" t="s">
+        <v>24</v>
+      </c>
+      <c r="F176" s="3">
+        <v>2.5710000000000002</v>
+      </c>
+    </row>
+    <row r="177" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B177" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="C177" t="s">
+        <v>93</v>
+      </c>
+      <c r="D177" t="s">
+        <v>92</v>
+      </c>
+      <c r="F177" s="3">
+        <v>5.2270000000000003</v>
+      </c>
+    </row>
+    <row r="178" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B178" s="2">
+        <v>8.1944444444444445E-2</v>
+      </c>
+      <c r="C178" t="s">
+        <v>85</v>
+      </c>
+      <c r="D178" t="s">
+        <v>92</v>
+      </c>
+      <c r="F178" s="3">
+        <v>11.3</v>
+      </c>
+      <c r="I178" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="179" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B179" s="2">
+        <v>0.12222222222222223</v>
+      </c>
+      <c r="C179" t="s">
+        <v>94</v>
+      </c>
+      <c r="D179" t="s">
+        <v>24</v>
+      </c>
+      <c r="F179" s="3">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="180" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B180" s="2">
+        <v>0.12638888888888888</v>
+      </c>
+      <c r="C180" t="s">
+        <v>94</v>
+      </c>
+      <c r="D180" t="s">
+        <v>24</v>
+      </c>
+      <c r="F180" s="3">
+        <v>3.2829999999999999</v>
+      </c>
+    </row>
+    <row r="181" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B181" s="2">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="C181" t="s">
+        <v>94</v>
+      </c>
+      <c r="D181" t="s">
+        <v>24</v>
+      </c>
+      <c r="F181" s="3">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="182" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B182" s="2">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="C182" t="s">
+        <v>96</v>
+      </c>
+      <c r="D182" t="s">
+        <v>24</v>
+      </c>
+      <c r="F182" s="3">
+        <v>3.0680000000000001</v>
+      </c>
+    </row>
+    <row r="183" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B183" s="2">
+        <v>0.20972222222222223</v>
+      </c>
+      <c r="C183" t="s">
+        <v>94</v>
+      </c>
+      <c r="D183" t="s">
+        <v>24</v>
+      </c>
+      <c r="F183" s="3">
+        <v>2.8780000000000001</v>
+      </c>
+    </row>
+    <row r="184" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B184" s="2">
+        <v>0.21041666666666667</v>
+      </c>
+      <c r="C184" t="s">
+        <v>93</v>
+      </c>
+      <c r="D184" t="s">
+        <v>92</v>
+      </c>
+      <c r="F184" s="3">
+        <v>4.7210000000000001</v>
+      </c>
+    </row>
+    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B185" s="2">
+        <v>0.22777777777777777</v>
+      </c>
+      <c r="C185" t="s">
+        <v>97</v>
+      </c>
+      <c r="D185" t="s">
+        <v>24</v>
+      </c>
+      <c r="F185" s="3">
+        <v>3.097</v>
+      </c>
+    </row>
+    <row r="186" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B186" s="2">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="C186" t="s">
+        <v>97</v>
+      </c>
+      <c r="D186" t="s">
+        <v>24</v>
+      </c>
+      <c r="F186" s="3">
+        <v>2.919</v>
+      </c>
+    </row>
+    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B187" s="2">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="C187" t="s">
+        <v>94</v>
+      </c>
+      <c r="D187" t="s">
+        <v>92</v>
+      </c>
+      <c r="F187" s="3">
+        <v>2.964</v>
+      </c>
+    </row>
+    <row r="188" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B188" s="2">
+        <v>0.28402777777777777</v>
+      </c>
+      <c r="C188" t="s">
+        <v>98</v>
+      </c>
+      <c r="D188" t="s">
+        <v>24</v>
+      </c>
+      <c r="F188" s="3">
+        <v>2.7810000000000001</v>
+      </c>
+    </row>
+    <row r="189" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B189" s="2">
+        <v>0.28472222222222221</v>
+      </c>
+      <c r="C189" t="s">
+        <v>85</v>
+      </c>
+      <c r="D189" t="s">
+        <v>92</v>
+      </c>
+      <c r="F189" s="3">
+        <v>8.5220000000000002</v>
+      </c>
+    </row>
+    <row r="190" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B190" s="2">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="C190" t="s">
+        <v>93</v>
+      </c>
+      <c r="D190" t="s">
+        <v>92</v>
+      </c>
+      <c r="F190" s="3">
+        <v>6.9640000000000004</v>
+      </c>
+    </row>
+    <row r="191" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B191" s="2">
+        <v>0.8222222222222223</v>
+      </c>
+      <c r="C191" t="s">
+        <v>93</v>
+      </c>
+      <c r="D191" t="s">
+        <v>92</v>
+      </c>
+      <c r="F191" s="3">
+        <v>3.8759999999999999</v>
+      </c>
+    </row>
+    <row r="192" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B192" s="2">
+        <v>0.83611111111111114</v>
+      </c>
+      <c r="C192" t="s">
+        <v>93</v>
+      </c>
+      <c r="D192" t="s">
+        <v>92</v>
+      </c>
+      <c r="F192" s="3">
+        <v>7.6230000000000002</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B193" s="2">
+        <v>0.87638888888888899</v>
+      </c>
+      <c r="C193" t="s">
+        <v>93</v>
+      </c>
+      <c r="D193" t="s">
+        <v>92</v>
+      </c>
+      <c r="F193" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B194" s="2">
+        <v>0.87708333333333333</v>
+      </c>
+      <c r="C194" t="s">
+        <v>94</v>
+      </c>
+      <c r="D194" t="s">
+        <v>24</v>
+      </c>
+      <c r="F194" s="3">
+        <v>1.6879999999999999</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B195" s="2">
+        <v>0.87777777777777777</v>
+      </c>
+      <c r="C195" t="s">
+        <v>98</v>
+      </c>
+      <c r="D195" t="s">
+        <v>24</v>
+      </c>
+      <c r="F195" s="3">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B196" s="2">
+        <v>0.87916666666666676</v>
+      </c>
+      <c r="C196" t="s">
+        <v>85</v>
+      </c>
+      <c r="D196" t="s">
+        <v>92</v>
+      </c>
+      <c r="F196" s="3">
+        <v>5.4089999999999998</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B197" s="2">
+        <v>0.8965277777777777</v>
+      </c>
+      <c r="C197" t="s">
+        <v>99</v>
+      </c>
+      <c r="D197" t="s">
+        <v>24</v>
+      </c>
+      <c r="F197" s="3">
+        <v>2.3889999999999998</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B198" s="2">
+        <v>0.8965277777777777</v>
+      </c>
+      <c r="C198" t="s">
+        <v>93</v>
+      </c>
+      <c r="D198" t="s">
+        <v>92</v>
+      </c>
+      <c r="F198" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B199" s="2">
+        <v>0.89722222222222225</v>
+      </c>
+      <c r="C199" t="s">
+        <v>94</v>
+      </c>
+      <c r="D199" t="s">
+        <v>24</v>
+      </c>
+      <c r="F199" s="3">
+        <v>2.4950000000000001</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B200" s="2">
+        <v>0.9590277777777777</v>
+      </c>
+      <c r="C200" t="s">
+        <v>100</v>
+      </c>
+      <c r="D200" t="s">
+        <v>24</v>
+      </c>
+      <c r="F200" s="3">
+        <v>3.7690000000000001</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B201" s="2">
+        <v>0.9590277777777777</v>
+      </c>
+      <c r="C201" t="s">
+        <v>93</v>
+      </c>
+      <c r="D201" t="s">
+        <v>92</v>
+      </c>
+      <c r="F201" s="3">
+        <v>5.8150000000000004</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B202" s="2">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="C202" t="s">
+        <v>85</v>
+      </c>
+      <c r="D202" t="s">
+        <v>92</v>
+      </c>
+      <c r="F202" s="3">
+        <v>8.7609999999999992</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A203" s="1">
+        <v>45742</v>
+      </c>
+      <c r="B203" s="2">
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="C203" t="s">
+        <v>100</v>
+      </c>
+      <c r="D203" t="s">
+        <v>24</v>
+      </c>
+      <c r="F203" s="3">
+        <v>3.9830000000000001</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B204" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C204" t="s">
+        <v>93</v>
+      </c>
+      <c r="D204" t="s">
+        <v>92</v>
+      </c>
+      <c r="F204" s="3">
+        <v>6.6790000000000003</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B205" s="2">
+        <v>0.75694444444444453</v>
+      </c>
+      <c r="C205" t="s">
+        <v>53</v>
+      </c>
+      <c r="D205" t="s">
+        <v>92</v>
+      </c>
+      <c r="F205" s="3">
+        <v>4.8520000000000003</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B206" s="2">
+        <v>0.75763888888888886</v>
+      </c>
+      <c r="C206" t="s">
+        <v>93</v>
+      </c>
+      <c r="D206" t="s">
+        <v>92</v>
+      </c>
+      <c r="F206" s="3">
+        <v>2.052</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B207" s="2">
+        <v>0.77847222222222223</v>
+      </c>
+      <c r="C207" t="s">
+        <v>93</v>
+      </c>
+      <c r="D207" t="s">
+        <v>92</v>
+      </c>
+      <c r="F207" s="3">
+        <v>4.9589999999999996</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B208" s="2">
+        <v>0.79583333333333339</v>
+      </c>
+      <c r="C208" t="s">
+        <v>93</v>
+      </c>
+      <c r="D208" t="s">
+        <v>92</v>
+      </c>
+      <c r="F208" s="3">
+        <v>5.9870000000000001</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B209" s="2">
+        <v>0.79583333333333339</v>
+      </c>
+      <c r="C209" t="s">
+        <v>93</v>
+      </c>
+      <c r="D209" t="s">
+        <v>101</v>
+      </c>
+      <c r="F209" s="3">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="210" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B210" s="2">
+        <v>0.79652777777777783</v>
+      </c>
+      <c r="C210" t="s">
+        <v>93</v>
+      </c>
+      <c r="D210" t="s">
+        <v>10</v>
+      </c>
+      <c r="F210" s="3">
+        <v>5.37</v>
+      </c>
+    </row>
+    <row r="211" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B211" s="2">
+        <v>0.8041666666666667</v>
+      </c>
+      <c r="C211" t="s">
+        <v>93</v>
+      </c>
+      <c r="D211" t="s">
+        <v>92</v>
+      </c>
+      <c r="F211" s="3">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="212" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B212" s="2">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="C212" t="s">
+        <v>93</v>
+      </c>
+      <c r="D212" t="s">
+        <v>92</v>
+      </c>
+      <c r="F212" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="213" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B213" s="2">
+        <v>0.85277777777777775</v>
+      </c>
+      <c r="C213" t="s">
+        <v>93</v>
+      </c>
+      <c r="D213" t="s">
+        <v>92</v>
+      </c>
+      <c r="F213" s="3">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="214" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B214" s="2">
+        <v>0.8534722222222223</v>
+      </c>
+      <c r="C214" t="s">
+        <v>53</v>
+      </c>
+      <c r="D214" t="s">
+        <v>92</v>
+      </c>
+      <c r="F214" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="215" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B215" s="2">
+        <v>0.85486111111111107</v>
+      </c>
+      <c r="C215" t="s">
+        <v>102</v>
+      </c>
+      <c r="D215" t="s">
+        <v>92</v>
+      </c>
+      <c r="F215" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="216" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B216" s="2">
+        <v>0.85763888888888884</v>
+      </c>
+      <c r="C216" t="s">
+        <v>103</v>
+      </c>
+      <c r="D216" t="s">
+        <v>92</v>
+      </c>
+      <c r="F216" s="3">
+        <v>12.3</v>
+      </c>
+      <c r="I216" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="217" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B217" s="2">
+        <v>0.87083333333333324</v>
+      </c>
+      <c r="C217" t="s">
+        <v>104</v>
+      </c>
+      <c r="D217" t="s">
+        <v>10</v>
+      </c>
+      <c r="F217" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="218" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B218" s="2">
+        <v>0.87986111111111109</v>
+      </c>
+      <c r="C218" t="s">
+        <v>93</v>
+      </c>
+      <c r="D218" t="s">
+        <v>10</v>
+      </c>
+      <c r="F218" s="3">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="219" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B219" s="2">
+        <v>0.88680555555555562</v>
+      </c>
+      <c r="C219" t="s">
+        <v>105</v>
+      </c>
+      <c r="D219" t="s">
+        <v>10</v>
+      </c>
+      <c r="F219" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="220" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B220" s="2">
+        <v>0.93611111111111101</v>
+      </c>
+      <c r="C220" t="s">
+        <v>126</v>
+      </c>
+      <c r="D220" t="s">
+        <v>10</v>
+      </c>
+      <c r="F220" s="3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="221" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B221" s="2">
+        <v>0.93819444444444444</v>
+      </c>
+      <c r="C221" t="s">
+        <v>106</v>
+      </c>
+      <c r="D221" t="s">
+        <v>10</v>
+      </c>
+      <c r="F221" s="3">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="222" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B222" s="2">
+        <v>0.94305555555555554</v>
+      </c>
+      <c r="C222" t="s">
+        <v>127</v>
+      </c>
+      <c r="D222" t="s">
+        <v>10</v>
+      </c>
+      <c r="F222" s="3">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="223" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B223" s="2">
+        <v>0.9458333333333333</v>
+      </c>
+      <c r="C223" t="s">
+        <v>106</v>
+      </c>
+      <c r="D223" t="s">
+        <v>10</v>
+      </c>
+      <c r="F223" s="3">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="224" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B224" s="2">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="C224" t="s">
+        <v>128</v>
+      </c>
+      <c r="D224" t="s">
+        <v>107</v>
+      </c>
+      <c r="F224" s="3">
+        <f>69.73/8</f>
+        <v>8.7162500000000005</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B225" s="2">
+        <v>0.95277777777777783</v>
+      </c>
+      <c r="C225" t="s">
+        <v>129</v>
+      </c>
+      <c r="D225" t="s">
+        <v>107</v>
+      </c>
+      <c r="F225" s="3">
+        <f>78.14/8</f>
+        <v>9.7675000000000001</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B226" s="2">
+        <v>0.95347222222222217</v>
+      </c>
+      <c r="C226" t="s">
+        <v>130</v>
+      </c>
+      <c r="D226" t="s">
+        <v>107</v>
+      </c>
+      <c r="F226" s="3">
+        <f>106.12/8</f>
+        <v>13.265000000000001</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B227" s="2">
+        <v>0.99861111111111101</v>
+      </c>
+      <c r="C227" t="s">
+        <v>126</v>
+      </c>
+      <c r="D227" t="s">
+        <v>10</v>
+      </c>
+      <c r="F227" s="3">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B228" s="2">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="C228" t="s">
+        <v>128</v>
+      </c>
+      <c r="D228" t="s">
+        <v>107</v>
+      </c>
+      <c r="F228" s="3">
+        <f>76.68/8</f>
+        <v>9.5850000000000009</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A229" s="1">
+        <v>45743</v>
+      </c>
+      <c r="B229" s="2">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="C229" t="s">
+        <v>131</v>
+      </c>
+      <c r="D229" t="s">
+        <v>10</v>
+      </c>
+      <c r="F229" s="3">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B230" s="2">
+        <v>0.87083333333333324</v>
+      </c>
+      <c r="C230" t="s">
+        <v>132</v>
+      </c>
+      <c r="D230" t="s">
+        <v>10</v>
+      </c>
+      <c r="F230" s="3">
+        <v>13</v>
+      </c>
+      <c r="I230" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B231" s="2">
+        <v>0.87291666666666667</v>
+      </c>
+      <c r="C231" t="s">
+        <v>133</v>
+      </c>
+      <c r="D231" t="s">
+        <v>10</v>
+      </c>
+      <c r="F231" s="3">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B232" s="2">
+        <v>0.90138888888888891</v>
+      </c>
+      <c r="C232" t="s">
+        <v>108</v>
+      </c>
+      <c r="D232" t="s">
+        <v>10</v>
+      </c>
+      <c r="F232" s="3">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B233" s="2">
+        <v>0.91875000000000007</v>
+      </c>
+      <c r="C233" t="s">
+        <v>132</v>
+      </c>
+      <c r="D233" t="s">
+        <v>10</v>
+      </c>
+      <c r="F233" s="3">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B234" s="2">
+        <v>0.92013888888888884</v>
+      </c>
+      <c r="C234" t="s">
+        <v>128</v>
+      </c>
+      <c r="D234" t="s">
+        <v>107</v>
+      </c>
+      <c r="F234" s="3">
+        <f>69.21/8</f>
+        <v>8.6512499999999992</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A235" s="1">
+        <v>45744</v>
+      </c>
+      <c r="B235" s="2">
+        <v>0.10208333333333335</v>
+      </c>
+      <c r="C235" t="s">
+        <v>134</v>
+      </c>
+      <c r="D235" t="s">
+        <v>10</v>
+      </c>
+      <c r="F235" s="3">
+        <v>6.37</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B236" s="2">
+        <v>0.12638888888888888</v>
+      </c>
+      <c r="C236" t="s">
+        <v>134</v>
+      </c>
+      <c r="D236" t="s">
+        <v>10</v>
+      </c>
+      <c r="F236" s="3">
+        <v>9.2899999999999991</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B237" s="2">
+        <v>0.12638888888888888</v>
+      </c>
+      <c r="C237" t="s">
+        <v>93</v>
+      </c>
+      <c r="D237" t="s">
+        <v>10</v>
+      </c>
+      <c r="F237" s="3">
+        <v>8.51</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B238" s="2">
+        <v>0.84930555555555554</v>
+      </c>
+      <c r="C238" t="s">
+        <v>93</v>
+      </c>
+      <c r="D238" t="s">
+        <v>10</v>
+      </c>
+      <c r="F238" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B239" s="2">
+        <v>0.8520833333333333</v>
+      </c>
+      <c r="C239" t="s">
+        <v>93</v>
+      </c>
+      <c r="D239" t="s">
+        <v>10</v>
+      </c>
+      <c r="F239" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B240" s="2">
+        <v>0.8520833333333333</v>
+      </c>
+      <c r="C240" t="s">
+        <v>134</v>
+      </c>
+      <c r="D240" t="s">
+        <v>10</v>
+      </c>
+      <c r="F240" s="3">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="241" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B241" s="2">
+        <v>0.8534722222222223</v>
+      </c>
+      <c r="C241" t="s">
+        <v>134</v>
+      </c>
+      <c r="D241" t="s">
+        <v>21</v>
+      </c>
+      <c r="F241" s="3">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="242" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B242" s="2">
+        <v>0.8534722222222223</v>
+      </c>
+      <c r="C242" t="s">
+        <v>135</v>
+      </c>
+      <c r="D242" t="s">
+        <v>10</v>
+      </c>
+      <c r="F242" s="3">
+        <v>9.14</v>
+      </c>
+    </row>
+    <row r="243" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B243" s="2">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="C243" t="s">
+        <v>93</v>
+      </c>
+      <c r="D243" t="s">
+        <v>10</v>
+      </c>
+      <c r="F243" s="3">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="244" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B244" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C244" t="s">
+        <v>44</v>
+      </c>
+      <c r="D244" t="s">
+        <v>10</v>
+      </c>
+      <c r="F244" s="3">
+        <v>15.3</v>
+      </c>
+      <c r="I244" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="245" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B245" s="2">
+        <v>3.4027777777777775E-2</v>
+      </c>
+      <c r="C245" t="s">
+        <v>90</v>
+      </c>
+      <c r="D245" t="s">
+        <v>109</v>
+      </c>
+      <c r="F245" s="3">
+        <f>1000/70</f>
+        <v>14.285714285714286</v>
+      </c>
+    </row>
+    <row r="246" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B246" s="2">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="C246" t="s">
+        <v>136</v>
+      </c>
+      <c r="D246" t="s">
+        <v>10</v>
+      </c>
+      <c r="F246" s="3">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="247" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B247" s="2">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="C247" t="s">
+        <v>137</v>
+      </c>
+      <c r="D247" t="s">
+        <v>10</v>
+      </c>
+      <c r="F247" s="3">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="248" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B248" s="2">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="C248" t="s">
+        <v>110</v>
+      </c>
+      <c r="D248" t="s">
+        <v>10</v>
+      </c>
+      <c r="F248" s="3">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="249" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B249" s="2">
+        <v>5.1388888888888894E-2</v>
+      </c>
+      <c r="C249" t="s">
+        <v>111</v>
+      </c>
+      <c r="D249" t="s">
+        <v>10</v>
+      </c>
+      <c r="F249" s="3">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="250" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B250" s="2">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="C250" t="s">
+        <v>112</v>
+      </c>
+      <c r="D250" t="s">
+        <v>10</v>
+      </c>
+      <c r="F250" s="3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="251" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B251" s="2">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="C251" t="s">
+        <v>113</v>
+      </c>
+      <c r="D251" t="s">
+        <v>10</v>
+      </c>
+      <c r="F251" s="3">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="252" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B252" s="2">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="C252" t="s">
+        <v>138</v>
+      </c>
+      <c r="D252" t="s">
+        <v>10</v>
+      </c>
+      <c r="F252" s="3">
+        <v>0.748</v>
+      </c>
+    </row>
+    <row r="253" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B253" s="2">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="C253" t="s">
+        <v>137</v>
+      </c>
+      <c r="D253" t="s">
+        <v>10</v>
+      </c>
+      <c r="F253" s="3">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="254" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B254" s="2">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="C254" t="s">
+        <v>128</v>
+      </c>
+      <c r="D254" t="s">
+        <v>107</v>
+      </c>
+      <c r="F254" s="3">
+        <f>73.58/8</f>
+        <v>9.1974999999999998</v>
+      </c>
+    </row>
+    <row r="255" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B255" s="2">
+        <v>5.9027777777777783E-2</v>
+      </c>
+      <c r="C255" t="s">
+        <v>139</v>
+      </c>
+      <c r="D255" t="s">
+        <v>10</v>
+      </c>
+      <c r="F255" s="3">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="256" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B256" s="2">
+        <v>6.1111111111111116E-2</v>
+      </c>
+      <c r="C256" t="s">
+        <v>130</v>
+      </c>
+      <c r="D256" t="s">
+        <v>107</v>
+      </c>
+      <c r="F256" s="3">
+        <f>88.96/8</f>
+        <v>11.12</v>
+      </c>
+    </row>
+    <row r="257" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B257" s="2">
+        <v>0.20972222222222223</v>
+      </c>
+      <c r="C257" t="s">
+        <v>130</v>
+      </c>
+      <c r="D257" t="s">
+        <v>107</v>
+      </c>
+      <c r="F257" s="3">
+        <f>75.49/8</f>
+        <v>9.4362499999999994</v>
+      </c>
+    </row>
+    <row r="258" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B258" s="2">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="C258" t="s">
+        <v>128</v>
+      </c>
+      <c r="D258" t="s">
+        <v>10</v>
+      </c>
+      <c r="E258">
+        <v>100</v>
+      </c>
+      <c r="F258" s="3">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="259" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B259" s="2">
+        <v>0.21458333333333335</v>
+      </c>
+      <c r="C259" t="s">
+        <v>128</v>
+      </c>
+      <c r="D259" t="s">
+        <v>10</v>
+      </c>
+      <c r="F259" s="3">
+        <v>7.49</v>
+      </c>
+    </row>
+    <row r="260" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B260" s="2">
+        <v>0.21527777777777779</v>
+      </c>
+      <c r="C260" t="s">
+        <v>130</v>
+      </c>
+      <c r="D260" t="s">
+        <v>10</v>
+      </c>
+      <c r="F260" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="261" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B261" s="2">
+        <v>0.21527777777777779</v>
+      </c>
+      <c r="C261" t="s">
+        <v>130</v>
+      </c>
+      <c r="D261" t="s">
+        <v>10</v>
+      </c>
+      <c r="F261" s="3">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="262" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B262" s="2">
+        <v>0.21805555555555556</v>
+      </c>
+      <c r="C262" t="s">
+        <v>128</v>
+      </c>
+      <c r="D262" t="s">
+        <v>10</v>
+      </c>
+      <c r="F262" s="3">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="263" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B263" s="2">
+        <v>0.21875</v>
+      </c>
+      <c r="C263" t="s">
+        <v>140</v>
+      </c>
+      <c r="D263" t="s">
+        <v>10</v>
+      </c>
+      <c r="F263" s="3">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="264" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B264" s="2">
+        <v>0.21944444444444444</v>
+      </c>
+      <c r="C264" t="s">
+        <v>93</v>
+      </c>
+      <c r="D264" t="s">
+        <v>10</v>
+      </c>
+      <c r="F264" s="3">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="265" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B265" s="2">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C265" t="s">
+        <v>141</v>
+      </c>
+      <c r="D265" t="s">
+        <v>10</v>
+      </c>
+      <c r="F265" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="266" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B266" s="2">
+        <v>0.22569444444444445</v>
+      </c>
+      <c r="C266" t="s">
+        <v>142</v>
+      </c>
+      <c r="D266" t="s">
+        <v>10</v>
+      </c>
+      <c r="F266" s="3">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="267" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B267" s="2">
+        <v>0.22638888888888889</v>
+      </c>
+      <c r="C267" t="s">
+        <v>143</v>
+      </c>
+      <c r="D267" t="s">
+        <v>10</v>
+      </c>
+      <c r="F267" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="268" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B268" s="2">
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="C268" t="s">
+        <v>144</v>
+      </c>
+      <c r="D268" t="s">
+        <v>10</v>
+      </c>
+      <c r="F268" s="3">
+        <v>8.11</v>
+      </c>
+    </row>
+    <row r="269" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B269" s="2">
+        <v>0.22777777777777777</v>
+      </c>
+      <c r="C269" t="s">
+        <v>145</v>
+      </c>
+      <c r="D269" t="s">
+        <v>10</v>
+      </c>
+      <c r="F269" s="3">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="270" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B270" s="2">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="C270" t="s">
+        <v>146</v>
+      </c>
+      <c r="D270" t="s">
+        <v>10</v>
+      </c>
+      <c r="F270" s="3">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="271" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B271" s="2">
+        <v>0.23055555555555554</v>
+      </c>
+      <c r="C271" t="s">
+        <v>147</v>
+      </c>
+      <c r="D271" t="s">
+        <v>10</v>
+      </c>
+      <c r="F271" s="3">
+        <v>8.51</v>
+      </c>
+      <c r="I271" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="272" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B272" s="2">
+        <v>0.23124999999999998</v>
+      </c>
+      <c r="C272" t="s">
+        <v>114</v>
+      </c>
+      <c r="D272" t="s">
+        <v>10</v>
+      </c>
+      <c r="F272" s="3">
+        <v>84</v>
+      </c>
+      <c r="I272" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B273" s="2">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="C273" t="s">
+        <v>147</v>
+      </c>
+      <c r="D273" t="s">
+        <v>10</v>
+      </c>
+      <c r="F273" s="3">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B274" s="2">
+        <v>0.23333333333333331</v>
+      </c>
+      <c r="C274" t="s">
+        <v>140</v>
+      </c>
+      <c r="D274" t="s">
+        <v>10</v>
+      </c>
+      <c r="F274" s="3">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B275" s="2">
+        <v>0.23402777777777781</v>
+      </c>
+      <c r="C275" t="s">
+        <v>116</v>
+      </c>
+      <c r="D275" t="s">
+        <v>101</v>
+      </c>
+      <c r="F275" s="3">
+        <v>12</v>
+      </c>
+      <c r="I275" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B276" s="2">
+        <v>0.23402777777777781</v>
+      </c>
+      <c r="C276" t="s">
+        <v>116</v>
+      </c>
+      <c r="D276" t="s">
+        <v>101</v>
+      </c>
+      <c r="F276" s="3">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B277" s="2">
+        <v>0.23819444444444446</v>
+      </c>
+      <c r="C277" t="s">
+        <v>137</v>
+      </c>
+      <c r="D277" t="s">
+        <v>101</v>
+      </c>
+      <c r="F277" s="3">
+        <v>7.13</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B278" s="2">
+        <v>0.23819444444444446</v>
+      </c>
+      <c r="C278" t="s">
+        <v>137</v>
+      </c>
+      <c r="D278" t="s">
+        <v>101</v>
+      </c>
+      <c r="F278" s="3">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A279" s="1">
+        <v>45748</v>
+      </c>
+      <c r="B279" s="2">
+        <v>0.78888888888888886</v>
+      </c>
+      <c r="C279" t="s">
+        <v>147</v>
+      </c>
+      <c r="D279" t="s">
+        <v>10</v>
+      </c>
+      <c r="F279" s="3">
+        <v>9.4499999999999993</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B280" s="2">
+        <v>0.7895833333333333</v>
+      </c>
+      <c r="C280" t="s">
+        <v>116</v>
+      </c>
+      <c r="D280" t="s">
+        <v>101</v>
+      </c>
+      <c r="F280" s="3">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B281" s="2">
+        <v>0.79027777777777775</v>
+      </c>
+      <c r="C281" t="s">
+        <v>119</v>
+      </c>
+      <c r="D281" t="s">
+        <v>10</v>
+      </c>
+      <c r="F281" s="3">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B282" s="2">
+        <v>0.7909722222222223</v>
+      </c>
+      <c r="C282" t="s">
+        <v>137</v>
+      </c>
+      <c r="D282" t="s">
+        <v>101</v>
+      </c>
+      <c r="F282" s="3">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B283" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="C283" t="s">
+        <v>150</v>
+      </c>
+      <c r="D283" t="s">
+        <v>10</v>
+      </c>
+      <c r="F283" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B284" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="C284" t="s">
+        <v>137</v>
+      </c>
+      <c r="D284" t="s">
+        <v>101</v>
+      </c>
+      <c r="F284" s="3">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B285" s="2">
+        <v>0.97569444444444453</v>
+      </c>
+      <c r="C285" t="s">
+        <v>116</v>
+      </c>
+      <c r="D285" t="s">
+        <v>101</v>
+      </c>
+      <c r="F285" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B286" s="2">
+        <v>0.9770833333333333</v>
+      </c>
+      <c r="C286" t="s">
+        <v>119</v>
+      </c>
+      <c r="D286" t="s">
+        <v>101</v>
+      </c>
+      <c r="F286" s="3">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A287" s="1">
+        <v>45759</v>
+      </c>
+      <c r="B287" s="2">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="C287" t="s">
+        <v>148</v>
+      </c>
+      <c r="D287" t="s">
+        <v>120</v>
+      </c>
+      <c r="F287" s="3">
+        <f>158.59/8</f>
+        <v>19.82375</v>
+      </c>
+      <c r="H287" s="4">
+        <f>2.52/8</f>
+        <v>0.315</v>
+      </c>
+      <c r="I287" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B288" s="2">
+        <v>0.90347222222222223</v>
+      </c>
+      <c r="C288" t="s">
+        <v>122</v>
+      </c>
+      <c r="D288" t="s">
+        <v>120</v>
+      </c>
+      <c r="F288" s="3">
+        <f>0.94/8</f>
+        <v>0.11749999999999999</v>
+      </c>
+      <c r="H288" s="4">
+        <f>2.86/8</f>
+        <v>0.35749999999999998</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B289" s="2">
+        <v>0.90902777777777777</v>
+      </c>
+      <c r="C289" t="s">
+        <v>123</v>
+      </c>
+      <c r="D289" t="s">
+        <v>120</v>
+      </c>
+      <c r="F289" s="3">
+        <f>152.3/8</f>
+        <v>19.037500000000001</v>
+      </c>
+      <c r="H289" s="4">
+        <f>2.7/8</f>
+        <v>0.33750000000000002</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A290" s="1">
+        <v>45762</v>
+      </c>
+      <c r="B290" s="2">
+        <v>0.61527777777777781</v>
+      </c>
+      <c r="C290" t="s">
+        <v>124</v>
+      </c>
+      <c r="D290" t="s">
+        <v>120</v>
+      </c>
+      <c r="F290" s="3">
+        <f>193.03/8</f>
+        <v>24.12875</v>
+      </c>
+      <c r="H290" s="4">
+        <f>4.46/8</f>
+        <v>0.5575</v>
+      </c>
+      <c r="I290" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B291" s="2">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="C291" t="s">
+        <v>93</v>
+      </c>
+      <c r="D291" t="s">
+        <v>125</v>
+      </c>
+      <c r="H291" s="4">
+        <f>10.1/(7.74+7.09+0.225)</f>
+        <v>0.67087346396545999</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A292" s="1">
+        <v>45774</v>
+      </c>
+      <c r="B292" s="2">
+        <v>0.6743055555555556</v>
+      </c>
+      <c r="C292" t="s">
+        <v>149</v>
+      </c>
+      <c r="D292" t="s">
+        <v>10</v>
+      </c>
+      <c r="F292" s="3">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A293" s="1">
+        <v>45782</v>
+      </c>
+      <c r="B293" s="2">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="C293" t="s">
+        <v>152</v>
+      </c>
+      <c r="D293" t="s">
+        <v>10</v>
+      </c>
+      <c r="F293" s="3">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A294" s="1">
+        <v>45782</v>
+      </c>
+      <c r="B294" s="2">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="C294" t="s">
+        <v>151</v>
+      </c>
+      <c r="D294" t="s">
+        <v>10</v>
+      </c>
+      <c r="F294" s="3">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A295" s="1">
+        <v>45782</v>
+      </c>
+      <c r="B295" s="2">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="C295" t="s">
+        <v>154</v>
+      </c>
+      <c r="D295" t="s">
+        <v>153</v>
+      </c>
+      <c r="F295" s="3">
+        <f>27.5/(49*60+14-(48*60+8))</f>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B296" s="2">
+        <v>0.72291666666666676</v>
+      </c>
+      <c r="C296" t="s">
+        <v>155</v>
+      </c>
+      <c r="D296" t="s">
+        <v>153</v>
+      </c>
+      <c r="F296" s="3">
+        <f>27.5/(21*60+52-(21*60+47))</f>
+        <v>5.5</v>
+      </c>
+      <c r="I296" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B297" s="2">
+        <v>0.7284722222222223</v>
+      </c>
+      <c r="C297" t="s">
+        <v>156</v>
+      </c>
+      <c r="D297" t="s">
+        <v>153</v>
+      </c>
+      <c r="F297" s="3">
+        <f>13/(0.348+0.731+0.108)</f>
+        <v>10.951979780960404</v>
+      </c>
+      <c r="I297" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B298" s="2">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="C298" t="s">
+        <v>158</v>
+      </c>
+      <c r="D298" t="s">
+        <v>153</v>
+      </c>
+      <c r="F298" s="3">
+        <f>27.5/(34*60+59-(34*60+48))</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B299" s="2">
+        <v>0.74861111111111101</v>
+      </c>
+      <c r="C299" t="s">
+        <v>159</v>
+      </c>
+      <c r="D299" t="s">
+        <v>153</v>
+      </c>
+      <c r="F299" s="3">
+        <f>27.5/(31-8)</f>
+        <v>1.1956521739130435</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B300" s="2">
+        <v>0.75277777777777777</v>
+      </c>
+      <c r="C300" t="s">
+        <v>159</v>
+      </c>
+      <c r="D300" t="s">
+        <v>153</v>
+      </c>
+      <c r="F300" s="3">
+        <f>27.5/(67-47)</f>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B301" s="2">
+        <v>0.75486111111111109</v>
+      </c>
+      <c r="C301" t="s">
+        <v>158</v>
+      </c>
+      <c r="D301" t="s">
+        <v>153</v>
+      </c>
+      <c r="F301" s="3">
+        <f>27.5/(64-54)</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B302" s="2">
+        <v>0.75555555555555554</v>
+      </c>
+      <c r="C302" t="s">
+        <v>154</v>
+      </c>
+      <c r="D302" t="s">
+        <v>153</v>
+      </c>
+      <c r="F302" s="3">
+        <f>27.5/(60+47-44)</f>
+        <v>0.43650793650793651</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B303" s="2">
+        <v>0.79027777777777775</v>
+      </c>
+      <c r="C303" t="s">
+        <v>159</v>
+      </c>
+      <c r="D303" t="s">
+        <v>153</v>
+      </c>
+      <c r="F303" s="3">
+        <f>27.5/(31-13)</f>
+        <v>1.5277777777777777</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B304" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C304" t="s">
+        <v>160</v>
+      </c>
+      <c r="D304" t="s">
+        <v>153</v>
+      </c>
+      <c r="F304" s="3">
+        <f>27.5/10</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A305" s="1">
+        <v>45826</v>
+      </c>
+      <c r="B305" s="2">
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="C305" t="s">
+        <v>161</v>
+      </c>
+      <c r="D305" t="s">
+        <v>10</v>
+      </c>
+      <c r="F305" s="3">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B306" s="2">
+        <v>0.96875</v>
+      </c>
+      <c r="C306" t="s">
+        <v>163</v>
+      </c>
+      <c r="D306" t="s">
+        <v>10</v>
+      </c>
+      <c r="F306" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B307" s="2">
+        <v>0.97013888888888899</v>
+      </c>
+      <c r="C307" t="s">
+        <v>162</v>
+      </c>
+      <c r="D307" t="s">
+        <v>10</v>
+      </c>
+      <c r="E307">
+        <v>100</v>
+      </c>
+      <c r="F307" s="3">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B308" s="2">
+        <v>0.97083333333333333</v>
+      </c>
+      <c r="C308" t="s">
+        <v>161</v>
+      </c>
+      <c r="D308" t="s">
+        <v>10</v>
+      </c>
+      <c r="F308" s="3">
+        <v>9.32</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B309" s="2">
+        <v>0.97569444444444453</v>
+      </c>
+      <c r="C309" t="s">
+        <v>175</v>
+      </c>
+      <c r="D309" t="s">
+        <v>176</v>
+      </c>
+      <c r="F309" s="3">
+        <f>75.09/8</f>
+        <v>9.3862500000000004</v>
+      </c>
+      <c r="H309" s="4">
+        <f>3.01/8</f>
+        <v>0.37624999999999997</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C310" t="s">
+        <v>174</v>
+      </c>
+      <c r="D310" t="s">
+        <v>176</v>
+      </c>
+      <c r="F310" s="3">
+        <f>77.51/8</f>
+        <v>9.6887500000000006</v>
+      </c>
+      <c r="H310" s="4">
+        <f>38.55/8</f>
+        <v>4.8187499999999996</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B311" s="2">
+        <v>0.97638888888888886</v>
+      </c>
+      <c r="C311" t="s">
+        <v>163</v>
+      </c>
+      <c r="D311" t="s">
+        <v>176</v>
+      </c>
+      <c r="F311" s="3">
+        <f>98.21/8</f>
+        <v>12.276249999999999</v>
+      </c>
+      <c r="H311" s="4">
+        <f>2.61/8</f>
+        <v>0.32624999999999998</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C312" t="s">
+        <v>161</v>
+      </c>
+      <c r="D312" t="s">
+        <v>176</v>
+      </c>
+      <c r="F312" s="3">
+        <f>128.62/8</f>
+        <v>16.077500000000001</v>
+      </c>
+      <c r="H312" s="4">
+        <f>38.43/8</f>
+        <v>4.80375</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C313" t="s">
+        <v>164</v>
+      </c>
+      <c r="D313" t="s">
+        <v>176</v>
+      </c>
+      <c r="F313" s="3">
+        <f>1.85/8</f>
+        <v>0.23125000000000001</v>
+      </c>
+      <c r="H313" s="4">
+        <f>21.83/8</f>
+        <v>2.7287499999999998</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C314" t="s">
+        <v>165</v>
+      </c>
+      <c r="D314" t="s">
+        <v>176</v>
+      </c>
+      <c r="F314" s="3">
+        <f>3.99/8</f>
+        <v>0.49875000000000003</v>
+      </c>
+      <c r="H314" s="4">
+        <f>3.77/8</f>
+        <v>0.47125</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C315" t="s">
+        <v>166</v>
+      </c>
+      <c r="D315" t="s">
+        <v>176</v>
+      </c>
+      <c r="F315" s="3">
+        <f>147.32/8</f>
+        <v>18.414999999999999</v>
+      </c>
+      <c r="H315" s="4">
+        <f>23.26/8</f>
+        <v>2.9075000000000002</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C316" t="s">
+        <v>167</v>
+      </c>
+      <c r="D316" t="s">
+        <v>176</v>
+      </c>
+      <c r="F316" s="3">
+        <f>106.46/8</f>
+        <v>13.307499999999999</v>
+      </c>
+      <c r="H316" s="4">
+        <f>30.32/8</f>
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C317" t="s">
+        <v>162</v>
+      </c>
+      <c r="D317" t="s">
+        <v>176</v>
+      </c>
+      <c r="F317" s="3">
+        <f>13.82/8</f>
+        <v>1.7275</v>
+      </c>
+      <c r="H317" s="4">
+        <f>25.28/8</f>
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C318" t="s">
+        <v>168</v>
+      </c>
+      <c r="D318" t="s">
+        <v>176</v>
+      </c>
+      <c r="F318" s="3">
+        <f>3.69/8</f>
+        <v>0.46124999999999999</v>
+      </c>
+      <c r="H318" s="4">
+        <f>30.3/8</f>
+        <v>3.7875000000000001</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B319" s="2">
+        <v>0.98125000000000007</v>
+      </c>
+      <c r="C319" t="s">
+        <v>169</v>
+      </c>
+      <c r="D319" t="s">
+        <v>176</v>
+      </c>
+      <c r="F319" s="3">
+        <f>156.02/8</f>
+        <v>19.502500000000001</v>
+      </c>
+      <c r="H319" s="4">
+        <f>29.05/8</f>
+        <v>3.6312500000000001</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B320" s="2">
+        <v>0.99375000000000002</v>
+      </c>
+      <c r="C320" t="s">
+        <v>171</v>
+      </c>
+      <c r="D320" t="s">
+        <v>10</v>
+      </c>
+      <c r="F320" s="3">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="321" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C321" t="s">
+        <v>170</v>
+      </c>
+      <c r="D321" t="s">
+        <v>10</v>
+      </c>
+      <c r="F321" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="322" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C322" t="s">
+        <v>172</v>
+      </c>
+      <c r="D322" t="s">
+        <v>10</v>
+      </c>
+      <c r="F322" s="3">
+        <v>45.2</v>
+      </c>
+    </row>
+    <row r="323" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C323" t="s">
+        <v>173</v>
+      </c>
+      <c r="D323" t="s">
+        <v>10</v>
+      </c>
+      <c r="F323" s="3">
+        <v>9.23</v>
+      </c>
+    </row>
+    <row r="324" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A324" s="1">
+        <v>45827</v>
+      </c>
+      <c r="B324" s="2">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="C324" t="s">
+        <v>177</v>
+      </c>
+      <c r="D324" t="s">
+        <v>176</v>
+      </c>
+      <c r="F324" s="3">
+        <f>397.87/8</f>
+        <v>49.733750000000001</v>
+      </c>
+      <c r="H324" s="4">
+        <f>54.75/8</f>
+        <v>6.84375</v>
+      </c>
+    </row>
+    <row r="325" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C325" t="s">
+        <v>178</v>
+      </c>
+      <c r="D325" t="s">
+        <v>176</v>
+      </c>
+      <c r="F325" s="3">
+        <f>39.04/8</f>
+        <v>4.88</v>
+      </c>
+      <c r="H325" s="4">
+        <f>26.73/8</f>
+        <v>3.3412500000000001</v>
+      </c>
+    </row>
+    <row r="326" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B326" s="2">
+        <v>9.5138888888888884E-2</v>
+      </c>
+      <c r="C326" t="s">
+        <v>161</v>
+      </c>
+      <c r="D326" t="s">
+        <v>176</v>
+      </c>
+      <c r="F326" s="3">
+        <f>0.39/8</f>
+        <v>4.8750000000000002E-2</v>
+      </c>
+      <c r="H326" s="4">
+        <f>32.37/8</f>
+        <v>4.0462499999999997</v>
+      </c>
+    </row>
+    <row r="327" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C327" t="s">
+        <v>163</v>
+      </c>
+      <c r="D327" t="s">
+        <v>176</v>
+      </c>
+      <c r="F327" s="3">
+        <f>182.92/8</f>
+        <v>22.864999999999998</v>
+      </c>
+      <c r="H327" s="4">
+        <f>39.7/8</f>
+        <v>4.9625000000000004</v>
+      </c>
+    </row>
+    <row r="328" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A328" s="1">
+        <v>45827</v>
+      </c>
+      <c r="B328" s="2">
+        <v>0.90694444444444444</v>
+      </c>
+      <c r="C328" t="s">
+        <v>42</v>
+      </c>
+      <c r="D328" t="s">
+        <v>10</v>
+      </c>
+      <c r="F328" s="3">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="329" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C329" t="s">
+        <v>93</v>
+      </c>
+      <c r="D329" t="s">
+        <v>10</v>
+      </c>
+      <c r="F329" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B330" s="2">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="C330" t="s">
+        <v>179</v>
+      </c>
+      <c r="D330" t="s">
+        <v>10</v>
+      </c>
+      <c r="F330" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C331" t="s">
+        <v>93</v>
+      </c>
+      <c r="D331" t="s">
+        <v>10</v>
+      </c>
+      <c r="F331" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="332" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A332" s="1">
+        <v>45830</v>
+      </c>
+      <c r="B332" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="C332" t="s">
+        <v>180</v>
+      </c>
+      <c r="D332" t="s">
+        <v>10</v>
+      </c>
+      <c r="E332">
+        <v>100</v>
+      </c>
+      <c r="F332" s="3">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C333" t="s">
+        <v>181</v>
+      </c>
+      <c r="D333" t="s">
+        <v>10</v>
+      </c>
+      <c r="E333">
+        <v>100</v>
+      </c>
+      <c r="F333" s="3">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="334" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B334" s="2">
+        <v>0.84652777777777777</v>
+      </c>
+      <c r="C334" t="s">
+        <v>182</v>
+      </c>
+      <c r="D334" t="s">
+        <v>10</v>
+      </c>
+      <c r="E334">
+        <v>100</v>
+      </c>
+      <c r="F334" s="3">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B335" s="2">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="C335" t="s">
+        <v>180</v>
+      </c>
+      <c r="D335" t="s">
+        <v>10</v>
+      </c>
+      <c r="E335">
+        <v>100</v>
+      </c>
+      <c r="F335" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="I335" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="336" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C336" t="s">
+        <v>181</v>
+      </c>
+      <c r="D336" t="s">
+        <v>10</v>
+      </c>
+      <c r="E336">
+        <v>100</v>
+      </c>
+      <c r="F336" s="3">
+        <v>13.7</v>
+      </c>
+      <c r="I336" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A337" s="1">
+        <v>45849</v>
+      </c>
+      <c r="B337" s="2">
+        <v>0.81874999999999998</v>
+      </c>
+      <c r="C337" t="s">
+        <v>44</v>
+      </c>
+      <c r="D337" t="s">
+        <v>10</v>
+      </c>
+      <c r="E337">
+        <v>100</v>
+      </c>
+      <c r="F337" s="3">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B338" s="2">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="C338" t="s">
+        <v>42</v>
+      </c>
+      <c r="D338" t="s">
+        <v>10</v>
+      </c>
+      <c r="E338">
+        <v>100</v>
+      </c>
+      <c r="F338" s="3">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A339" s="1">
+        <v>45911</v>
+      </c>
+      <c r="B339" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C339" t="s">
+        <v>44</v>
+      </c>
+      <c r="D339" t="s">
+        <v>10</v>
+      </c>
+      <c r="E339">
+        <v>100</v>
+      </c>
+      <c r="F339" s="3">
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B340" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C340" t="s">
+        <v>185</v>
+      </c>
+      <c r="D340" t="s">
+        <v>10</v>
+      </c>
+      <c r="E340">
+        <v>100</v>
+      </c>
+      <c r="F340" s="3">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="341" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B341" s="2">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C341" t="s">
+        <v>44</v>
+      </c>
+      <c r="D341" t="s">
+        <v>10</v>
+      </c>
+      <c r="E341">
+        <v>100</v>
+      </c>
+      <c r="F341" s="3">
+        <v>4.6100000000000003</v>
+      </c>
+    </row>
+    <row r="342" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B342" s="2">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="C342" t="s">
+        <v>186</v>
+      </c>
+      <c r="D342" t="s">
+        <v>10</v>
+      </c>
+      <c r="E342">
+        <v>100</v>
+      </c>
+      <c r="F342" s="3">
+        <v>9.6199999999999992</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B343" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C343" t="s">
+        <v>42</v>
+      </c>
+      <c r="D343" t="s">
+        <v>10</v>
+      </c>
+      <c r="E343">
+        <v>100</v>
+      </c>
+      <c r="F343" s="3">
+        <v>4.1399999999999997</v>
+      </c>
+    </row>
+    <row r="344" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A344" s="1">
+        <v>45914</v>
+      </c>
+      <c r="B344" s="2">
+        <v>0.93333333333333324</v>
+      </c>
+      <c r="C344" t="s">
+        <v>42</v>
+      </c>
+      <c r="D344" t="s">
+        <v>10</v>
+      </c>
+      <c r="E344">
+        <v>100</v>
+      </c>
+      <c r="F344" s="3">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="I344" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="345" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B345" s="2">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="C345" t="s">
+        <v>44</v>
+      </c>
+      <c r="D345" t="s">
+        <v>10</v>
+      </c>
+      <c r="E345">
+        <v>100</v>
+      </c>
+      <c r="F345" s="3">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="I345" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="346" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B346" s="2">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="C346" t="s">
+        <v>185</v>
+      </c>
+      <c r="D346" t="s">
+        <v>10</v>
+      </c>
+      <c r="E346">
+        <v>100</v>
+      </c>
+      <c r="F346" s="3">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B347" s="2">
+        <v>0.97986111111111107</v>
+      </c>
+      <c r="C347" t="s">
+        <v>186</v>
+      </c>
+      <c r="D347" t="s">
+        <v>10</v>
+      </c>
+      <c r="E347">
+        <v>100</v>
+      </c>
+      <c r="F347" s="3">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="348" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B348" s="2">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="C348" t="s">
+        <v>44</v>
+      </c>
+      <c r="D348" t="s">
+        <v>10</v>
+      </c>
+      <c r="E348">
+        <v>100</v>
+      </c>
+      <c r="F348" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="I348" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="349" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B349" s="2">
+        <v>0.98749999999999993</v>
+      </c>
+      <c r="C349" t="s">
+        <v>42</v>
+      </c>
+      <c r="D349" t="s">
+        <v>10</v>
+      </c>
+      <c r="E349">
+        <v>100</v>
+      </c>
+      <c r="F349" s="3">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="I349" t="s">
+        <v>187</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="F1:F86 F93:F130 F132:F1048576 H1:H102 H109:H1048576">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F130 F132:F1048576 H131">
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="num" val="20"/>
         <color rgb="FFFFEF9C"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
@@ -2902,6 +6310,14 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H142">
     <cfRule type="colorScale" priority="2">

</xml_diff>